<commit_message>
Fix for selection the option for catlog search
</commit_message>
<xml_diff>
--- a/test_results/suggest_3_books_for_childrens.xlsx
+++ b/test_results/suggest_3_books_for_childrens.xlsx
@@ -431,53 +431,53 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Books for Children</v>
+        <v>Books for children</v>
       </c>
       <c r="B2" t="str">
-        <v>The Antiracist Kid</v>
+        <v>Henry Huggins</v>
       </c>
       <c r="C2" t="str">
-        <v>The book is tailored for young readers | It guides young readers like Ruby, Shawn, and Dani | The book aims to empower young readers by teaching them about identity, justice, and activism</v>
+        <v>The book is a classic | It features an average boy whose life is turned upside down when he meets a lovable puppy with a nose for mischief | The book falls under the genre of JUVENILE FICTION</v>
       </c>
       <c r="D2" t="str">
-        <v>98%</v>
+        <v>100%</v>
       </c>
       <c r="E2" t="str">
-        <v>The relevance score is 98% because while the book is highly relevant to children, its focus on antiracism may not align with all interpretations of general children's books.</v>
+        <v>No gap mentioned</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Books for Children</v>
+        <v>Books for children</v>
       </c>
       <c r="B3" t="str">
-        <v>Axel the Truck: Rocky Road</v>
+        <v>Anne of Green Gables</v>
       </c>
       <c r="C3" t="str">
-        <v>The book is specifically designed as an "I Can Read Book" | It features full-color art | The book is about Axel, a little truck with great big wheels</v>
+        <v>The book is a classic | It features a talkative eleven-year-old orphan with a heart full of dreams and a desperate longing for a home | The book falls under the genre of JUVENILE FICTION</v>
       </c>
       <c r="D3" t="str">
-        <v>95%</v>
+        <v>100%</v>
       </c>
       <c r="E3" t="str">
-        <v>The relevance score is 95% because while the book is designed for children, its focus on trucks and reading skills may not align with all interpretations of general children's books.</v>
+        <v>No gap mentioned</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Books for Children</v>
+        <v>Books for children</v>
       </c>
       <c r="B4" t="str">
-        <v>Fancy Nancy: Hair Dos and Hair Dont's</v>
+        <v>The Secret Garden</v>
       </c>
       <c r="C4" t="str">
-        <v>The book is part of the Fancy Nancy I Can Read series | It is designed for children learning to sound out words and sentences | The book features a comical and endearing story about Fancy Nancy</v>
+        <v>The book is a classic | It features an orphaned girl who discovers a secret garden and brings it back to life | The book falls under the genre of JUVENILE FICTION</v>
       </c>
       <c r="D4" t="str">
-        <v>93%</v>
+        <v>100%</v>
       </c>
       <c r="E4" t="str">
-        <v>The relevance score is 93% because while the book is designed for children, its focus on Fancy Nancy and hair styling may not align with all interpretations of general children's books.</v>
+        <v>No gap mentioned</v>
       </c>
     </row>
   </sheetData>

</xml_diff>